<commit_message>
Saving Changes before I try to start editing for the Wash Performance Lab
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Washer DOE/Documentation/Building 1 Lab IP Assignment.xlsx
+++ b/NI-2010/Trunk/Washer DOE/Documentation/Building 1 Lab IP Assignment.xlsx
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="883">
   <si>
     <t>Station</t>
   </si>
@@ -2641,6 +2641,102 @@
   </si>
   <si>
     <t>192.168.1.35</t>
+  </si>
+  <si>
+    <t>192.168.3.1</t>
+  </si>
+  <si>
+    <t>192.168.3.2</t>
+  </si>
+  <si>
+    <t>192.168.3.3</t>
+  </si>
+  <si>
+    <t>192.168.3.4</t>
+  </si>
+  <si>
+    <t>192.168.3.5</t>
+  </si>
+  <si>
+    <t>192.168.3.6</t>
+  </si>
+  <si>
+    <t>192.168.3.7</t>
+  </si>
+  <si>
+    <t>192.168.3.8</t>
+  </si>
+  <si>
+    <t>192.168.3.9</t>
+  </si>
+  <si>
+    <t>192.168.3.10</t>
+  </si>
+  <si>
+    <t>192.168.3.11</t>
+  </si>
+  <si>
+    <t>192.168.3.12</t>
+  </si>
+  <si>
+    <t>192.168.3.13</t>
+  </si>
+  <si>
+    <t>192.168.3.14</t>
+  </si>
+  <si>
+    <t>192.168.3.15</t>
+  </si>
+  <si>
+    <t>192.168.3.16</t>
+  </si>
+  <si>
+    <t>192.168.3.17</t>
+  </si>
+  <si>
+    <t>192.168.3.18</t>
+  </si>
+  <si>
+    <t>192.168.3.19</t>
+  </si>
+  <si>
+    <t>192.168.3.20</t>
+  </si>
+  <si>
+    <t>192.168.3.21</t>
+  </si>
+  <si>
+    <t>192.168.3.22</t>
+  </si>
+  <si>
+    <t>192.168.3.23</t>
+  </si>
+  <si>
+    <t>Wash Performance APLUS Station 1</t>
+  </si>
+  <si>
+    <t>Wash Perf Laurel Hot Temp St 1</t>
+  </si>
+  <si>
+    <t>Wash Perf Laurel Cold Temp St 1</t>
+  </si>
+  <si>
+    <t>Wash Perf Laurel Hot Pressure St 1</t>
+  </si>
+  <si>
+    <t>Wash Perf Laurel Cold Pressure St 1</t>
+  </si>
+  <si>
+    <t>Wash Perf Laurel Hot Flow St 1</t>
+  </si>
+  <si>
+    <t>Wash Perf Laurel Cold Flow St 1</t>
+  </si>
+  <si>
+    <t>Wash Performance PC???</t>
+  </si>
+  <si>
+    <t>Wash Performance 34972 Station 1</t>
   </si>
 </sst>
 </file>
@@ -15354,10 +15450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H349"/>
+  <dimension ref="A1:H377"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="A362" sqref="A362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20321,6 +20417,427 @@
       </c>
       <c r="B349" s="21"/>
     </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
+        <v>881</v>
+      </c>
+      <c r="B354" t="s">
+        <v>851</v>
+      </c>
+      <c r="C354">
+        <v>192</v>
+      </c>
+      <c r="D354">
+        <v>168</v>
+      </c>
+      <c r="E354">
+        <v>3</v>
+      </c>
+      <c r="F354">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
+        <v>875</v>
+      </c>
+      <c r="B355" s="15" t="s">
+        <v>852</v>
+      </c>
+      <c r="C355" s="15">
+        <v>192</v>
+      </c>
+      <c r="D355" s="15">
+        <v>168</v>
+      </c>
+      <c r="E355" s="15">
+        <v>3</v>
+      </c>
+      <c r="F355">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>876</v>
+      </c>
+      <c r="B356" s="15" t="s">
+        <v>853</v>
+      </c>
+      <c r="C356" s="15">
+        <v>192</v>
+      </c>
+      <c r="D356" s="15">
+        <v>168</v>
+      </c>
+      <c r="E356" s="15">
+        <v>3</v>
+      </c>
+      <c r="F356">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A357" t="s">
+        <v>877</v>
+      </c>
+      <c r="B357" s="15" t="s">
+        <v>854</v>
+      </c>
+      <c r="C357" s="15">
+        <v>192</v>
+      </c>
+      <c r="D357" s="15">
+        <v>168</v>
+      </c>
+      <c r="E357" s="15">
+        <v>3</v>
+      </c>
+      <c r="F357">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A358" t="s">
+        <v>878</v>
+      </c>
+      <c r="B358" s="15" t="s">
+        <v>855</v>
+      </c>
+      <c r="C358" s="15">
+        <v>192</v>
+      </c>
+      <c r="D358" s="15">
+        <v>168</v>
+      </c>
+      <c r="E358" s="15">
+        <v>3</v>
+      </c>
+      <c r="F358">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A359" t="s">
+        <v>879</v>
+      </c>
+      <c r="B359" s="15" t="s">
+        <v>856</v>
+      </c>
+      <c r="C359" s="15">
+        <v>192</v>
+      </c>
+      <c r="D359" s="15">
+        <v>168</v>
+      </c>
+      <c r="E359" s="15">
+        <v>3</v>
+      </c>
+      <c r="F359">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A360" t="s">
+        <v>880</v>
+      </c>
+      <c r="B360" s="15" t="s">
+        <v>857</v>
+      </c>
+      <c r="C360" s="15">
+        <v>192</v>
+      </c>
+      <c r="D360" s="15">
+        <v>168</v>
+      </c>
+      <c r="E360" s="15">
+        <v>3</v>
+      </c>
+      <c r="F360">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A361" t="s">
+        <v>874</v>
+      </c>
+      <c r="B361" s="15" t="s">
+        <v>858</v>
+      </c>
+      <c r="C361" s="15">
+        <v>192</v>
+      </c>
+      <c r="D361" s="15">
+        <v>168</v>
+      </c>
+      <c r="E361" s="15">
+        <v>3</v>
+      </c>
+      <c r="F361">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A362" t="s">
+        <v>882</v>
+      </c>
+      <c r="B362" s="15" t="s">
+        <v>859</v>
+      </c>
+      <c r="C362" s="15">
+        <v>192</v>
+      </c>
+      <c r="D362" s="15">
+        <v>168</v>
+      </c>
+      <c r="E362" s="15">
+        <v>3</v>
+      </c>
+      <c r="F362">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B363" s="15" t="s">
+        <v>860</v>
+      </c>
+      <c r="C363" s="15">
+        <v>192</v>
+      </c>
+      <c r="D363" s="15">
+        <v>168</v>
+      </c>
+      <c r="E363" s="15">
+        <v>3</v>
+      </c>
+      <c r="F363">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B364" s="15" t="s">
+        <v>861</v>
+      </c>
+      <c r="C364" s="15">
+        <v>192</v>
+      </c>
+      <c r="D364" s="15">
+        <v>168</v>
+      </c>
+      <c r="E364" s="15">
+        <v>3</v>
+      </c>
+      <c r="F364">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B365" s="15" t="s">
+        <v>862</v>
+      </c>
+      <c r="C365" s="15">
+        <v>192</v>
+      </c>
+      <c r="D365" s="15">
+        <v>168</v>
+      </c>
+      <c r="E365" s="15">
+        <v>3</v>
+      </c>
+      <c r="F365">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B366" s="15" t="s">
+        <v>863</v>
+      </c>
+      <c r="C366" s="15">
+        <v>192</v>
+      </c>
+      <c r="D366" s="15">
+        <v>168</v>
+      </c>
+      <c r="E366" s="15">
+        <v>3</v>
+      </c>
+      <c r="F366">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B367" s="15" t="s">
+        <v>864</v>
+      </c>
+      <c r="C367" s="15">
+        <v>192</v>
+      </c>
+      <c r="D367" s="15">
+        <v>168</v>
+      </c>
+      <c r="E367" s="15">
+        <v>3</v>
+      </c>
+      <c r="F367">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B368" s="15" t="s">
+        <v>865</v>
+      </c>
+      <c r="C368" s="15">
+        <v>192</v>
+      </c>
+      <c r="D368" s="15">
+        <v>168</v>
+      </c>
+      <c r="E368" s="15">
+        <v>3</v>
+      </c>
+      <c r="F368">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="369" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B369" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="C369" s="15">
+        <v>192</v>
+      </c>
+      <c r="D369" s="15">
+        <v>168</v>
+      </c>
+      <c r="E369" s="15">
+        <v>3</v>
+      </c>
+      <c r="F369">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="370" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B370" s="15" t="s">
+        <v>867</v>
+      </c>
+      <c r="C370" s="15">
+        <v>192</v>
+      </c>
+      <c r="D370" s="15">
+        <v>168</v>
+      </c>
+      <c r="E370" s="15">
+        <v>3</v>
+      </c>
+      <c r="F370">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="371" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B371" s="15" t="s">
+        <v>868</v>
+      </c>
+      <c r="C371" s="15">
+        <v>192</v>
+      </c>
+      <c r="D371" s="15">
+        <v>168</v>
+      </c>
+      <c r="E371" s="15">
+        <v>3</v>
+      </c>
+      <c r="F371">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="372" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B372" s="15" t="s">
+        <v>869</v>
+      </c>
+      <c r="C372" s="15">
+        <v>192</v>
+      </c>
+      <c r="D372" s="15">
+        <v>168</v>
+      </c>
+      <c r="E372" s="15">
+        <v>3</v>
+      </c>
+      <c r="F372">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="373" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B373" s="15" t="s">
+        <v>870</v>
+      </c>
+      <c r="C373" s="15">
+        <v>192</v>
+      </c>
+      <c r="D373" s="15">
+        <v>168</v>
+      </c>
+      <c r="E373" s="15">
+        <v>3</v>
+      </c>
+      <c r="F373">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="374" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B374" s="15" t="s">
+        <v>871</v>
+      </c>
+      <c r="C374" s="15">
+        <v>192</v>
+      </c>
+      <c r="D374" s="15">
+        <v>168</v>
+      </c>
+      <c r="E374" s="15">
+        <v>3</v>
+      </c>
+      <c r="F374">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="375" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B375" s="15" t="s">
+        <v>872</v>
+      </c>
+      <c r="C375" s="15">
+        <v>192</v>
+      </c>
+      <c r="D375" s="15">
+        <v>168</v>
+      </c>
+      <c r="E375" s="15">
+        <v>3</v>
+      </c>
+      <c r="F375">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="376" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B376" s="15" t="s">
+        <v>873</v>
+      </c>
+      <c r="C376" s="15">
+        <v>192</v>
+      </c>
+      <c r="D376" s="15">
+        <v>168</v>
+      </c>
+      <c r="E376" s="15">
+        <v>3</v>
+      </c>
+      <c r="F376">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="377" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E377" s="15"/>
+    </row>
   </sheetData>
   <sortState ref="A2:F102">
     <sortCondition ref="C2:C102"/>

</xml_diff>